<commit_message>
Flujo actualizado crear RRAA 15/09
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
+++ b/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FramerworkTsoft\Wappe\Web_automation_Wappe_AgenteMovistar\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A291CA3D-CC46-44A6-BFA9-256D74817F9D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15435FAF-69AB-4E32-9CDF-6079ED6E8D0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}" yWindow="-108"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" r:id="rId1" sheetId="1"/>
-    <sheet name="RRAA" r:id="rId2" sheetId="2"/>
-    <sheet name="Datos" r:id="rId3" sheetId="3"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="RRAA" sheetId="2" r:id="rId2"/>
+    <sheet name="Datos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>TC1</t>
   </si>
@@ -56,9 +56,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>EMPRESA CAJAS</t>
-  </si>
-  <si>
     <t>Roles</t>
   </si>
   <si>
@@ -84,14 +81,37 @@
   </si>
   <si>
     <t>Empleado</t>
+  </si>
+  <si>
+    <t>TIPO_DOCUMENTO</t>
+  </si>
+  <si>
+    <t>Tipo Documento</t>
+  </si>
+  <si>
+    <t>DNI</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>TipoDocumento</t>
+  </si>
+  <si>
+    <t>AJENICARAGUA S.A.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,71 +125,6 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <color indexed="17"/>
     </font>
   </fonts>
   <fills count="2">
@@ -205,35 +160,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0"/>
-    <xf applyFont="true" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -250,10 +199,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -288,7 +237,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -340,7 +289,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -451,21 +400,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -482,7 +431,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -534,112 +483,230 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E498FDF-C698-4C33-AB0D-10A8071429DC}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E498FDF-C698-4C33-AB0D-10A8071429DC}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" customWidth="true" width="44.21875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.88671875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>72402708</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink display="c0ntr@señ@" r:id="rId1" ref="D2" xr:uid="{DE3F403A-122E-426B-8B96-E38F4E9DE85F}"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3FD7F7-685D-489F-94C1-4B1D3A484504}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.44140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="2" max="2" width="40.21875" style="4" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.77734375" style="4" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.88671875" style="4" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.88671875" style="4" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>74542683</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>72402708</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3">
+        <v>72402708</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list" xr:uid="{47AA227F-BDA9-4E24-803B-338885745757}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AFF5B5F8-634A-4883-AA29-1C7792D93EA7}">
+          <x14:formula1>
+            <xm:f>Datos!$E$7:$E$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3FD7F7-685D-489F-94C1-4B1D3A484504}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="24.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1">
+        <v>74542683</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47AA227F-BDA9-4E24-803B-338885745757}">
           <x14:formula1>
             <xm:f>Datos!$C$7:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>D2</xm:sqref>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5A9E09E9-02E6-4968-AB62-5D7A9209FA89}">
+          <x14:formula1>
+            <xm:f>Datos!$E$7:$E$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -648,65 +715,84 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD572A2-87EF-411F-8B36-6BFC13510EDD}">
-  <dimension ref="C6:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD572A2-87EF-411F-8B36-6BFC13510EDD}">
+  <dimension ref="C5:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="23.77734375" collapsed="true"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+      <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Flujo RRAA con certificacion 16/09
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
+++ b/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FramerworkTsoft\Wappe\Web_automation_Wappe_AgenteMovistar\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15435FAF-69AB-4E32-9CDF-6079ED6E8D0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24322C3F-02DA-41B2-BD14-A0E997131A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="RRAA" sheetId="2" r:id="rId2"/>
-    <sheet name="Datos" sheetId="3" r:id="rId3"/>
+    <sheet name="Datos" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>TC1</t>
   </si>
@@ -53,9 +53,6 @@
     <t>NumDocumento</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>Roles</t>
   </si>
   <si>
@@ -104,14 +101,29 @@
     <t>TipoDocumento</t>
   </si>
   <si>
-    <t>AJENICARAGUA S.A.</t>
+    <t>EMPRESA PRUEBA</t>
+  </si>
+  <si>
+    <t>RolOnline</t>
+  </si>
+  <si>
+    <t>Rol Online</t>
+  </si>
+  <si>
+    <t>Decisor</t>
+  </si>
+  <si>
+    <t>Autorizado</t>
+  </si>
+  <si>
+    <t>Invitado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +137,14 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,10 +179,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -177,8 +198,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,7 +519,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +538,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -528,7 +553,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3">
         <v>72402708</v>
@@ -538,20 +563,23 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3">
-        <v>72402708</v>
+        <v>7240270</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" location="/agente" xr:uid="{C57B680B-9D45-4D3D-A8E0-847A9B51E02C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -570,10 +598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3FD7F7-685D-489F-94C1-4B1D3A484504}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,115 +615,160 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3">
         <v>74542683</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3">
+        <v>70622837</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47AA227F-BDA9-4E24-803B-338885745757}">
           <x14:formula1>
             <xm:f>Datos!$C$7:$C$14</xm:f>
@@ -708,6 +781,12 @@
           </x14:formula1>
           <xm:sqref>C1:C1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{45F83619-525B-44FB-80E1-E59769A0FD82}">
+          <x14:formula1>
+            <xm:f>Datos!$G$6:$G$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -716,10 +795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD572A2-87EF-411F-8B36-6BFC13510EDD}">
-  <dimension ref="C5:E14"/>
+  <dimension ref="C5:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,67 +807,79 @@
     <col min="5" max="5" width="29" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="G5" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+      <c r="G7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="2" t="s">
+      <c r="G8" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" s="2" t="s">
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C12" s="2" t="s">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C13" s="2" t="s">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flujo operaciones RRAA actualizado 06/10
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
+++ b/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FramerworkTsoft\Wappe\Web_automation_Wappe_AgenteMovistar\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24322C3F-02DA-41B2-BD14-A0E997131A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AA22A8-8E39-4987-BBF8-E86F8F9A5F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="RRAA" sheetId="2" r:id="rId2"/>
-    <sheet name="Datos" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="AnadirRRAA" sheetId="2" r:id="rId2"/>
+    <sheet name="EliminarRRAA" sheetId="4" r:id="rId3"/>
+    <sheet name="EditarRRAA" sheetId="5" r:id="rId4"/>
+    <sheet name="Datos" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>TC1</t>
   </si>
@@ -47,9 +49,6 @@
     <t>Peru567.</t>
   </si>
   <si>
-    <t>Empresa</t>
-  </si>
-  <si>
     <t>NumDocumento</t>
   </si>
   <si>
@@ -101,9 +100,6 @@
     <t>TipoDocumento</t>
   </si>
   <si>
-    <t>EMPRESA PRUEBA</t>
-  </si>
-  <si>
     <t>RolOnline</t>
   </si>
   <si>
@@ -117,6 +113,27 @@
   </si>
   <si>
     <t>Invitado</t>
+  </si>
+  <si>
+    <t>Lima2020.</t>
+  </si>
+  <si>
+    <t>RucEmpresa</t>
+  </si>
+  <si>
+    <t>CorreoCorporativo</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>RolComercial</t>
+  </si>
+  <si>
+    <t>20100041953</t>
+  </si>
+  <si>
+    <t>TC</t>
   </si>
 </sst>
 </file>
@@ -183,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -199,6 +216,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,7 +545,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +564,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -553,13 +579,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3">
-        <v>72402708</v>
+        <v>74542683</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -567,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3">
         <v>7240270</v>
@@ -598,170 +624,203 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3FD7F7-685D-489F-94C1-4B1D3A484504}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="24.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7">
+        <v>72297417</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7">
+        <v>70622837</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="3">
-        <v>74542683</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3">
-        <v>70622837</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -773,7 +832,7 @@
           <x14:formula1>
             <xm:f>Datos!$C$7:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5A9E09E9-02E6-4968-AB62-5D7A9209FA89}">
           <x14:formula1>
@@ -785,7 +844,7 @@
           <x14:formula1>
             <xm:f>Datos!$G$6:$G$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -794,6 +853,121 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FBCC37-EAAA-4CD0-A7F4-EF88531683C6}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="21.44140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7">
+        <v>72297417</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4215224A-B9DF-4B5A-B086-FD181311C5FE}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.21875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.6640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.5546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7">
+        <v>72297417</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D86B3167-F72C-47C2-BF48-39B4D4FBE305}">
+          <x14:formula1>
+            <xm:f>Datos!$G$6:$G$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1BDC7AA9-0132-453E-884B-3B6A10845AC2}">
+          <x14:formula1>
+            <xm:f>Datos!$C$7:$C$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD572A2-87EF-411F-8B36-6BFC13510EDD}">
   <dimension ref="C5:G14"/>
   <sheetViews>
@@ -810,76 +984,76 @@
     <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="E5" s="5"/>
       <c r="G5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatizacion Wappe Agente Actualizado 12/10
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
+++ b/src/main/resources/excel/DATA_WAPPE_MOVISTAR.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FramerworkTsoft\Wappe\Web_automation_Wappe_AgenteMovistar\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AA22A8-8E39-4987-BBF8-E86F8F9A5F11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5093AD29-D0DF-4F85-AFFA-0A6D3D76BFF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{2A2F275B-5F9E-4279-8630-EB21E5B75D93}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="AnadirRRAA" sheetId="2" r:id="rId2"/>
     <sheet name="EliminarRRAA" sheetId="4" r:id="rId3"/>
     <sheet name="EditarRRAA" sheetId="5" r:id="rId4"/>
-    <sheet name="Datos" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="CrearEmpresa" sheetId="6" r:id="rId5"/>
+    <sheet name="Datos" sheetId="3" state="hidden" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>TC1</t>
   </si>
@@ -115,32 +116,62 @@
     <t>Invitado</t>
   </si>
   <si>
+    <t>RucEmpresa</t>
+  </si>
+  <si>
+    <t>CorreoCorporativo</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>RolComercial</t>
+  </si>
+  <si>
+    <t>20100041953</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>peru124.</t>
+  </si>
+  <si>
+    <t>72402709</t>
+  </si>
+  <si>
+    <t>NumRUC</t>
+  </si>
+  <si>
+    <t>RazonSocial</t>
+  </si>
+  <si>
+    <t>Elpin SAC</t>
+  </si>
+  <si>
+    <t>74542683</t>
+  </si>
+  <si>
     <t>Lima2020.</t>
   </si>
   <si>
-    <t>RucEmpresa</t>
-  </si>
-  <si>
-    <t>CorreoCorporativo</t>
-  </si>
-  <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>RolComercial</t>
-  </si>
-  <si>
-    <t>20100041953</t>
-  </si>
-  <si>
-    <t>TC</t>
+    <t>20601567637</t>
+  </si>
+  <si>
+    <t>elpin2995@gmail.com</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>20480172111</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,13 +194,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -200,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -227,6 +270,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -542,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E498FDF-C698-4C33-AB0D-10A8071429DC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,16 +620,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
     </row>
@@ -581,11 +641,11 @@
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="3">
-        <v>74542683</v>
+      <c r="D2" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -596,10 +656,18 @@
         <v>18</v>
       </c>
       <c r="D3" s="3">
-        <v>7240270</v>
+        <v>72402709</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -624,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D3FD7F7-685D-489F-94C1-4B1D3A484504}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -638,53 +706,60 @@
     <col min="8" max="8" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="7">
-        <v>72297417</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
+        <v>41472468</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="7">
+        <v>979586095</v>
+      </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
@@ -703,7 +778,7 @@
       </c>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -716,7 +791,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -727,7 +802,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -738,7 +813,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -749,7 +824,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -760,7 +835,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -771,7 +846,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -782,7 +857,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -790,7 +865,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -798,7 +873,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -806,7 +881,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -814,7 +889,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -823,8 +898,11 @@
       <c r="G15" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{F2F81644-3E67-43A4-A895-93B1302B51C2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -854,10 +932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FBCC37-EAAA-4CD0-A7F4-EF88531683C6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -867,20 +945,25 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="7">
+        <v>41472468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="7">
         <v>72297417</v>
       </c>
     </row>
@@ -893,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4215224A-B9DF-4B5A-B086-FD181311C5FE}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,30 +992,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="7">
         <v>72297417</v>
@@ -968,6 +1051,54 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43029717-5E06-4F48-9969-6FEEA9FF0A84}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>20480172150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD572A2-87EF-411F-8B36-6BFC13510EDD}">
   <dimension ref="C5:G14"/>
   <sheetViews>

</xml_diff>